<commit_message>
Update example.xlsx file with data; create new empty file censuspopdata.xlsx
</commit_message>
<xml_diff>
--- a/workingWithExcelSpreadsheets/example.xlsx
+++ b/workingWithExcelSpreadsheets/example.xlsx
@@ -7,8 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet 3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -346,7 +347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +428,36 @@
       </c>
       <c r="C5" t="n">
         <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4/10/2015 6:10:37 PM</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bananas</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>4/10/2015 2:40:46 AM</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Strawberries</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -450,4 +481,22 @@
   <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>